<commit_message>
recheck and closed resolved issues
</commit_message>
<xml_diff>
--- a/exec/feedback of written testcases - symlex windows/test_cases/signup/signup username field.xlsx
+++ b/exec/feedback of written testcases - symlex windows/test_cases/signup/signup username field.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\office\SymlexVPNTestCases\exec\feedback of written testcases - symlex windows\test_cases\signup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4E560C-7B23-459C-A1FA-5527052882DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{059A2265-65F9-43E1-89C6-C8AC13EA6531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="163">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -663,6 +663,9 @@
   <si>
     <t>user@example.com#</t>
   </si>
+  <si>
+    <t>Input Data</t>
+  </si>
 </sst>
 </file>
 
@@ -864,7 +867,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -909,24 +912,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -956,6 +941,27 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1914,15 +1920,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="18"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="28"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1944,13 +1950,13 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="21"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="31"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -30033,7 +30039,7 @@
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -30042,290 +30048,292 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="32" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="2" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="23">
+      <c r="A2" s="17">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="19" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="23">
+      <c r="A3" s="17">
         <v>2</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A4" s="23">
+      <c r="A4" s="17">
         <v>3</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="20" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="23">
+      <c r="A5" s="17">
         <v>4</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="21" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="23">
+      <c r="A6" s="17">
         <v>5</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="21" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="23">
+      <c r="A7" s="17">
         <v>6</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="21" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="23">
+      <c r="A8" s="17">
         <v>7</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="21" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="23">
+      <c r="A9" s="17">
         <v>8</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="21" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="23">
+      <c r="A10" s="17">
         <v>9</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="21" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="23">
+      <c r="A11" s="17">
         <v>10</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="21" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="23">
+      <c r="A12" s="17">
         <v>11</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="21" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="23">
+      <c r="A13" s="17">
         <v>12</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="21" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="23">
+      <c r="A14" s="17">
         <v>13</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="21" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="23">
+      <c r="A15" s="17">
         <v>14</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="22" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="23">
+      <c r="A16" s="17">
         <v>15</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="21" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="23">
+      <c r="A17" s="17">
         <v>16</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="21" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="23">
+      <c r="A18" s="17">
         <v>17</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="22" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="23">
+      <c r="A19" s="17">
         <v>18</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="22" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="23">
+      <c r="A20" s="17">
         <v>19</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="22" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="23">
+      <c r="A21" s="17">
         <v>20</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="22" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="23">
+      <c r="A22" s="17">
         <v>21</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="22" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="23">
+      <c r="A23" s="17">
         <v>22</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="21" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="23">
+      <c r="A24" s="17">
         <v>23</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="22" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="23">
+      <c r="A25" s="17">
         <v>24</v>
       </c>
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="22" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="23">
+      <c r="A26" s="17">
         <v>25</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="22" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="30">
+      <c r="A27" s="24">
         <v>26</v>
       </c>
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="23" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="24">
+      <c r="A28" s="18">
         <v>27</v>
       </c>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="25" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="24">
+      <c r="A29" s="18">
         <v>28</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="25" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="24">
+      <c r="A30" s="18">
         <v>29</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="25" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="24">
+      <c r="A31" s="18">
         <v>30</v>
       </c>
-      <c r="B31" s="24"/>
+      <c r="B31" s="18"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="24">
+      <c r="A32" s="18">
         <v>31</v>
       </c>
-      <c r="B32" s="24"/>
+      <c r="B32" s="18"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="24">
+      <c r="A33" s="18">
         <v>32</v>
       </c>
-      <c r="B33" s="24"/>
+      <c r="B33" s="18"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="24">
+      <c r="A34" s="18">
         <v>33</v>
       </c>
-      <c r="B34" s="24"/>
+      <c r="B34" s="18"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="24">
+      <c r="A35" s="18">
         <v>34</v>
       </c>
-      <c r="B35" s="24"/>
+      <c r="B35" s="18"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="24">
+      <c r="A36" s="18">
         <v>35</v>
       </c>
-      <c r="B36" s="24"/>
+      <c r="B36" s="18"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="24"/>
-      <c r="B37" s="24"/>
+      <c r="A37" s="18"/>
+      <c r="B37" s="18"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="24"/>
-      <c r="B38" s="24"/>
+      <c r="A38" s="18"/>
+      <c r="B38" s="18"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="24"/>
-      <c r="B39" s="24"/>
+      <c r="A39" s="18"/>
+      <c r="B39" s="18"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>